<commit_message>
solved the problem with duplicates in frame_to_dict()
</commit_message>
<xml_diff>
--- a/archive of notifications DSO/test_file_old.xlsx
+++ b/archive of notifications DSO/test_file_old.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="360" windowWidth="23010" windowHeight="8970" tabRatio="717"/>
+    <workbookView xWindow="5610" yWindow="360" windowWidth="23010" windowHeight="8970" tabRatio="717"/>
   </bookViews>
   <sheets>
     <sheet name="31.05.22" sheetId="5" r:id="rId1"/>
@@ -514,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="49.9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -691,7 +691,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>10</v>
@@ -703,7 +703,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="11">
-        <v>44692</v>
+        <v>44772</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>10</v>
@@ -723,8 +723,14 @@
         <v>15</v>
       </c>
       <c r="F10" s="11">
-        <v>44042</v>
-      </c>
+        <v>44692</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:XFD2">

</xml_diff>